<commit_message>
Add Teleop arm control and update spreadsheet
Added Teleop arm control using the previously described "Set Arm Lift
Motor Output.vi" (this VI was also updated to provide dashboard values
and operate properly in simulations) and updated the robot control
assignments spreadsheet to include four drive motors (the robot code
must also be updated)
</commit_message>
<xml_diff>
--- a/2016 Stronghold Summer Robot Control Assignments roboRIO.xlsx
+++ b/2016 Stronghold Summer Robot Control Assignments roboRIO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>DIO</t>
   </si>
@@ -194,12 +194,6 @@
     <t>Upper Arm Switch?</t>
   </si>
   <si>
-    <t>Left Drive Motor Controller</t>
-  </si>
-  <si>
-    <t>Right Drive Motor Controller</t>
-  </si>
-  <si>
     <t>Left Weave Motor Controller</t>
   </si>
   <si>
@@ -237,6 +231,30 @@
   </si>
   <si>
     <t>*Used to detect whether the ball has fully entered the holding chamber</t>
+  </si>
+  <si>
+    <t>Left Front Drive Motor Controller</t>
+  </si>
+  <si>
+    <t>Right Front Drive Motor Controller</t>
+  </si>
+  <si>
+    <t>Left Rear Drive Motor Controller</t>
+  </si>
+  <si>
+    <t>Right Rear Drive Motor Controller</t>
+  </si>
+  <si>
+    <t>Left Front Drive Motor</t>
+  </si>
+  <si>
+    <t>Right Front Drive Motor</t>
+  </si>
+  <si>
+    <t>Left Rear Drive Motor</t>
+  </si>
+  <si>
+    <t>Right Rear Drive Motor</t>
   </si>
 </sst>
 </file>
@@ -446,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -470,9 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,19 +552,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -574,13 +577,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,7 +1077,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1084,39 +1099,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
+      <c r="A1" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
     </row>
     <row r="2" spans="1:14" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -1125,7 +1140,7 @@
       <c r="B3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5"/>
@@ -1135,14 +1150,14 @@
       <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="5"/>
@@ -1150,8 +1165,8 @@
         <v>2</v>
       </c>
       <c r="M3" s="6"/>
-      <c r="N3" s="61" t="s">
-        <v>62</v>
+      <c r="N3" s="47" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1161,8 +1176,8 @@
       <c r="B4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>70</v>
+      <c r="C4" s="46" t="s">
+        <v>68</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7">
@@ -1180,10 +1195,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" s="40" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="N4" s="39" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1212,9 +1227,9 @@
         <v>1</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="N5" s="40"/>
+        <v>71</v>
+      </c>
+      <c r="N5" s="39"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
@@ -1223,14 +1238,14 @@
       <c r="B6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="46" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="7">
         <v>2</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="10"/>
       <c r="H6" s="9"/>
       <c r="I6" s="7">
@@ -1241,10 +1256,10 @@
       <c r="L6" s="7">
         <v>2</v>
       </c>
-      <c r="M6" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" s="40"/>
+      <c r="M6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
@@ -1258,7 +1273,7 @@
       <c r="E7" s="7">
         <v>3</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="10"/>
       <c r="H7" s="9"/>
       <c r="I7" s="7">
@@ -1270,9 +1285,9 @@
         <v>3</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" s="40"/>
+        <v>73</v>
+      </c>
+      <c r="N7" s="39"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7">
@@ -1293,10 +1308,10 @@
       <c r="L8" s="7">
         <v>4</v>
       </c>
-      <c r="M8" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="N8" s="40"/>
+      <c r="M8" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="39"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
@@ -1305,7 +1320,7 @@
       <c r="B9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
@@ -1314,17 +1329,17 @@
       <c r="I9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="7">
         <v>5</v>
       </c>
-      <c r="M9" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="N9" s="40"/>
+      <c r="M9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="39"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
@@ -1342,17 +1357,17 @@
       <c r="I10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="7">
         <v>6</v>
       </c>
-      <c r="M10" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="40"/>
+      <c r="M10" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="39"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
@@ -1370,17 +1385,17 @@
       <c r="I11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="20" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="7">
         <v>7</v>
       </c>
-      <c r="M11" s="30" t="s">
+      <c r="M11" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="40"/>
+      <c r="N11" s="39"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
@@ -1401,8 +1416,10 @@
       <c r="L12" s="7">
         <v>8</v>
       </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="40"/>
+      <c r="M12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" s="39"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
@@ -1423,8 +1440,10 @@
       <c r="L13" s="7">
         <v>9</v>
       </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="40"/>
+      <c r="M13" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="N13" s="39"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
@@ -1433,7 +1452,7 @@
       <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="9"/>
@@ -1444,9 +1463,9 @@
       <c r="I14" s="7"/>
       <c r="J14" s="10"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="18"/>
+      <c r="L14" s="17"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="40"/>
+      <c r="N14" s="39"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
@@ -1455,7 +1474,7 @@
       <c r="B15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="9"/>
@@ -1466,9 +1485,9 @@
       <c r="I15" s="7"/>
       <c r="J15" s="10"/>
       <c r="K15" s="9"/>
-      <c r="L15" s="18"/>
+      <c r="L15" s="17"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="40"/>
+      <c r="N15" s="39"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
@@ -1477,7 +1496,7 @@
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="9"/>
@@ -1488,9 +1507,9 @@
       <c r="I16" s="7"/>
       <c r="J16" s="10"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="18"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="40"/>
+      <c r="N16" s="39"/>
     </row>
     <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7">
@@ -1499,20 +1518,20 @@
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="41"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="40"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
@@ -1521,78 +1540,78 @@
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="12">
+      <c r="A19" s="11">
         <v>15</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E20" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
+      <c r="E20" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:14" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="56"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="54" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="56"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="51"/>
     </row>
     <row r="22" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="24" t="s">
+      <c r="C22" s="53"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23" t="s">
+      <c r="K22" s="22"/>
+      <c r="L22" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="27" t="s">
+      <c r="M22" s="26" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1600,229 +1619,222 @@
       <c r="A23" s="7">
         <v>0</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
-      <c r="E23" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="28" t="s">
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="E23" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="J23" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" s="10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>1</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="49"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="28" t="s">
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J24" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M24" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>2</v>
       </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="28" t="s">
+      <c r="B25" s="58"/>
+      <c r="C25" s="59"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29" t="s">
+      <c r="J25" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M25" s="44" t="s">
-        <v>61</v>
+      <c r="M25" s="43" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>3</v>
       </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="28" t="s">
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29" t="s">
+      <c r="J26" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M26" s="30"/>
+      <c r="M26" s="29"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>4</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="49"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="28" t="s">
+      <c r="B27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29" t="s">
+      <c r="J27" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M27" s="30"/>
+      <c r="M27" s="29"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>5</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="49"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="28" t="s">
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="42"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29" t="s">
+      <c r="J28" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M28" s="30"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>6</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="49"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="28" t="s">
+      <c r="B29" s="58"/>
+      <c r="C29" s="59"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29" t="s">
+      <c r="J29" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="M29" s="30"/>
+      <c r="M29" s="29"/>
     </row>
     <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="7">
         <v>7</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="49"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="31" t="s">
+      <c r="B30" s="58"/>
+      <c r="C30" s="59"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32" t="s">
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="M30" s="33"/>
+      <c r="M30" s="32"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
+      <c r="C31" s="59"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
+      <c r="C32" s="61"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="I21:M21"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="E20:G22"/>
-    <mergeCell ref="E23:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
@@ -1836,6 +1848,17 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
+    <mergeCell ref="E23:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="E20:G22"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1862,136 +1885,136 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="40"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="15"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="14"/>
       <c r="G5" s="9"/>
     </row>
     <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="35">
+      <c r="B8" s="34">
         <v>1</v>
       </c>
-      <c r="C8" s="39"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="43">
+      <c r="B9" s="42">
         <f>B8+1</f>
         <v>2</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="43">
+      <c r="B10" s="42">
         <f t="shared" ref="B10:B18" si="0">B9+1</f>
         <v>3</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="35">
+      <c r="B11" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C11" s="40"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="35">
+      <c r="B12" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C12" s="40"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="35">
+      <c r="B13" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="35">
+      <c r="B14" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="35">
+      <c r="B15" s="34">
         <f>B14+1</f>
         <v>8</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="35">
+      <c r="B16" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="43">
+      <c r="B17" s="42">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C17" s="40"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="36">
+      <c r="B18" s="35">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="15"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2059,10 +2082,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="46"/>
+      <c r="B7" s="45"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Add "Ball Shooter Tasks.vi" and partial Teleop implementation
Added "Ball Shooter Tasks.vi" (only ball intake procedure has been
implemented; no testing has been completed)*; motor references in
Begin.vi have also been updated

*Joystick control for this procedure must still be added for Teleop
</commit_message>
<xml_diff>
--- a/2016 Stronghold Summer Robot Control Assignments roboRIO.xlsx
+++ b/2016 Stronghold Summer Robot Control Assignments roboRIO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
   <si>
     <t>DIO</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Right Rear Drive Motor</t>
+  </si>
+  <si>
+    <t>Winch Motor Controller</t>
   </si>
 </sst>
 </file>
@@ -555,6 +558,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,9 +587,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1076,8 +1079,8 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1099,39 +1102,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
     </row>
     <row r="2" spans="1:14" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -1308,8 +1311,8 @@
       <c r="L8" s="7">
         <v>4</v>
       </c>
-      <c r="M8" s="43" t="s">
-        <v>62</v>
+      <c r="M8" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="N8" s="39"/>
     </row>
@@ -1559,11 +1562,11 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
@@ -1572,34 +1575,34 @@
       <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:14" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="52"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="49" t="s">
+      <c r="I21" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="52"/>
     </row>
     <row r="22" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
+      <c r="C22" s="54"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
       <c r="H22" s="25"/>
       <c r="I22" s="23" t="s">
         <v>36</v>
@@ -1621,16 +1624,16 @@
       </c>
       <c r="B23" s="58"/>
       <c r="C23" s="59"/>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
       <c r="H23" s="25"/>
       <c r="I23" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="9" t="s">
         <v>74</v>
       </c>
       <c r="K23" s="28"/>
@@ -1647,14 +1650,14 @@
       </c>
       <c r="B24" s="58"/>
       <c r="C24" s="59"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
       <c r="H24" s="25"/>
       <c r="I24" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="9" t="s">
         <v>75</v>
       </c>
       <c r="K24" s="28"/>
@@ -1671,14 +1674,14 @@
       </c>
       <c r="B25" s="58"/>
       <c r="C25" s="59"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
       <c r="H25" s="25"/>
       <c r="I25" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="9" t="s">
         <v>76</v>
       </c>
       <c r="K25" s="28"/>
@@ -1695,14 +1698,14 @@
       </c>
       <c r="B26" s="58"/>
       <c r="C26" s="59"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
       <c r="H26" s="25"/>
       <c r="I26" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="9" t="s">
         <v>77</v>
       </c>
       <c r="K26" s="28"/>
@@ -1717,9 +1720,9 @@
       </c>
       <c r="B27" s="58"/>
       <c r="C27" s="59"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
       <c r="H27" s="25"/>
       <c r="I27" s="27" t="s">
         <v>35</v>
@@ -1739,9 +1742,9 @@
       </c>
       <c r="B28" s="58"/>
       <c r="C28" s="59"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
       <c r="H28" s="25"/>
       <c r="I28" s="27" t="s">
         <v>35</v>
@@ -1761,9 +1764,9 @@
       </c>
       <c r="B29" s="58"/>
       <c r="C29" s="59"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
       <c r="H29" s="25"/>
       <c r="I29" s="27" t="s">
         <v>35</v>
@@ -1783,9 +1786,9 @@
       </c>
       <c r="B30" s="58"/>
       <c r="C30" s="59"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
       <c r="H30" s="25"/>
       <c r="I30" s="30" t="s">
         <v>35</v>
@@ -1805,9 +1808,9 @@
         <v>28</v>
       </c>
       <c r="C31" s="59"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
@@ -1823,9 +1826,9 @@
         <v>30</v>
       </c>
       <c r="C32" s="61"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>

</xml_diff>

<commit_message>
Revise code to reflect current robot design and changes made during the competition and implement and revise vision processing
Revised the robot and dashboard code to reflect the current robot design
(code for the weave and winch was removed from the project*, motor
controller models were changed in Begin.vi, a camera ring light relay
switch was implemented, closed-loop automatic aiming was revised, and
spreadsheets were updated) and changes that were required during the
competition (fix drive system and other motor controls, update shooter
limit switch movement timeout, and change team number to the team number
that our second robot was registered under for this competition) and
implemented and revised dashboard vision processing.

*Weave VIs have been placed in "Other Robot Code"
</commit_message>
<xml_diff>
--- a/2016 Stronghold Summer Robot Control Assignments roboRIO.xlsx
+++ b/2016 Stronghold Summer Robot Control Assignments roboRIO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\2016-stronghold-summer-robot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="19140" windowHeight="9270"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Joystick Layout" sheetId="3" r:id="rId2"/>
     <sheet name="TechNotes" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
   <si>
     <t>DIO</t>
   </si>
@@ -188,30 +183,12 @@
     <t>SDA</t>
   </si>
   <si>
-    <t>Lower Arm Switch?</t>
-  </si>
-  <si>
-    <t>Upper Arm Switch?</t>
-  </si>
-  <si>
-    <t>Left Weave Motor Controller</t>
-  </si>
-  <si>
-    <t>Right Weave Motor Controller</t>
-  </si>
-  <si>
-    <t>Forward Weave Motor Controller</t>
-  </si>
-  <si>
     <t>MXP</t>
   </si>
   <si>
     <t>FRC ADI MXP IMU</t>
   </si>
   <si>
-    <t>Arm Lift Motor Controller</t>
-  </si>
-  <si>
     <t>Left Shooter Roller Controller</t>
   </si>
   <si>
@@ -221,9 +198,6 @@
     <t>Forward is defined by the direction that the ball shooter faces; Left and Right are defined as seen from behind the robot</t>
   </si>
   <si>
-    <t>Intake Weave Motor Controller</t>
-  </si>
-  <si>
     <t>2016 Summer HCRC Robot I/O - roboRIO</t>
   </si>
   <si>
@@ -233,38 +207,65 @@
     <t>*Used to detect whether the ball has fully entered the holding chamber</t>
   </si>
   <si>
-    <t>Left Front Drive Motor Controller</t>
-  </si>
-  <si>
-    <t>Right Front Drive Motor Controller</t>
-  </si>
-  <si>
-    <t>Left Rear Drive Motor Controller</t>
-  </si>
-  <si>
-    <t>Right Rear Drive Motor Controller</t>
-  </si>
-  <si>
-    <t>Left Front Drive Motor</t>
-  </si>
-  <si>
-    <t>Right Front Drive Motor</t>
-  </si>
-  <si>
-    <t>Left Rear Drive Motor</t>
-  </si>
-  <si>
-    <t>Right Rear Drive Motor</t>
-  </si>
-  <si>
-    <t>Winch Motor Controller</t>
+    <t>Shooter Lower Switch</t>
+  </si>
+  <si>
+    <t>Shooter Upper Switch</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>PDP</t>
+  </si>
+  <si>
+    <t>Left Shooter Roller</t>
+  </si>
+  <si>
+    <t>Right Shooter Roller</t>
+  </si>
+  <si>
+    <t>Right Drive Motor Controller</t>
+  </si>
+  <si>
+    <t>Left Drive Motor Controller</t>
+  </si>
+  <si>
+    <t>Left Drive Motor</t>
+  </si>
+  <si>
+    <t>Right Drive Motor</t>
+  </si>
+  <si>
+    <t>Arm Lift Motor</t>
+  </si>
+  <si>
+    <t>Lower Shooter Intake</t>
+  </si>
+  <si>
+    <t>Upper Shooter Intake</t>
+  </si>
+  <si>
+    <t>Camera Ring Light</t>
+  </si>
+  <si>
+    <t>Camera Right Light</t>
+  </si>
+  <si>
+    <t>Lower Shooter Intake Controller</t>
+  </si>
+  <si>
+    <t>Upper Shooter Intake Controller</t>
+  </si>
+  <si>
+    <t>Shooter Lift Controller</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,46 +559,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -830,7 +834,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -862,10 +866,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -897,7 +900,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1073,70 +1075,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="K16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="1.1796875" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1" customWidth="1"/>
-    <col min="12" max="12" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.08984375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33" customWidth="1"/>
+    <col min="14" max="14" width="1.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="16" max="16" width="1.140625" customWidth="1"/>
+    <col min="18" max="18" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-    </row>
-    <row r="2" spans="1:14" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="55" t="s">
+    <row r="1" spans="1:18" ht="21.75" thickBot="1">
+      <c r="A1" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+    </row>
+    <row r="2" spans="1:18" ht="21.75" thickBot="1">
+      <c r="A2" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1168,11 +1173,17 @@
         <v>2</v>
       </c>
       <c r="M3" s="6"/>
-      <c r="N3" s="47" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="N3" s="38"/>
+      <c r="O3" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="33"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="7">
         <v>0</v>
       </c>
@@ -1180,13 +1191,15 @@
         <v>33</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="G4" s="10"/>
       <c r="H4" s="9"/>
       <c r="I4" s="7">
@@ -1197,14 +1210,18 @@
       <c r="L4" s="7">
         <v>0</v>
       </c>
-      <c r="M4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M4" s="10"/>
+      <c r="O4" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>0</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -1212,7 +1229,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="7">
@@ -1229,12 +1246,16 @@
       <c r="L5" s="7">
         <v>1</v>
       </c>
-      <c r="M5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" s="39"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M5" s="10"/>
+      <c r="O5" s="39"/>
+      <c r="Q5" s="7">
+        <v>1</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -1242,7 +1263,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="7">
@@ -1260,11 +1281,17 @@
         <v>2</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="N6" s="39"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="O6" s="39"/>
+      <c r="Q6" s="7">
+        <v>2</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="7">
         <v>3</v>
       </c>
@@ -1287,12 +1314,14 @@
       <c r="L7" s="7">
         <v>3</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="N7" s="39"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M7" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="39"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="10"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1">
       <c r="A8" s="7">
         <v>4</v>
       </c>
@@ -1314,9 +1343,11 @@
       <c r="M8" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="N8" s="39"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O8" s="39"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -1339,12 +1370,14 @@
       <c r="L9" s="7">
         <v>5</v>
       </c>
-      <c r="M9" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N9" s="39"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M9" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="O9" s="39"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="10"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="7">
         <v>6</v>
       </c>
@@ -1367,12 +1400,14 @@
       <c r="L10" s="7">
         <v>6</v>
       </c>
-      <c r="M10" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="N10" s="39"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M10" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="39"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="10"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="7">
         <v>7</v>
       </c>
@@ -1395,12 +1430,11 @@
       <c r="L11" s="7">
         <v>7</v>
       </c>
-      <c r="M11" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="N11" s="39"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O11" s="39"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="10"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="7">
         <v>8</v>
       </c>
@@ -1419,12 +1453,12 @@
       <c r="L12" s="7">
         <v>8</v>
       </c>
-      <c r="M12" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="N12" s="39"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M12" s="10"/>
+      <c r="O12" s="39"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="10"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="7">
         <v>9</v>
       </c>
@@ -1443,12 +1477,12 @@
       <c r="L13" s="7">
         <v>9</v>
       </c>
-      <c r="M13" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" s="39"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M13" s="10"/>
+      <c r="O13" s="39"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="10"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="7">
         <v>10</v>
       </c>
@@ -1468,9 +1502,11 @@
       <c r="K14" s="9"/>
       <c r="L14" s="17"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="39"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O14" s="39"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="10"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="7">
         <v>11</v>
       </c>
@@ -1490,9 +1526,11 @@
       <c r="K15" s="9"/>
       <c r="L15" s="17"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="39"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O15" s="39"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="10"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="7">
         <v>12</v>
       </c>
@@ -1512,9 +1550,11 @@
       <c r="K16" s="9"/>
       <c r="L16" s="17"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="39"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O16" s="39"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="10"/>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" thickBot="1">
       <c r="A17" s="7">
         <v>13</v>
       </c>
@@ -1535,8 +1575,12 @@
       <c r="L17" s="18"/>
       <c r="M17" s="14"/>
       <c r="N17" s="40"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="14"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="7">
         <v>14</v>
       </c>
@@ -1547,7 +1591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" ht="15.75" thickBot="1">
       <c r="A19" s="11">
         <v>15</v>
       </c>
@@ -1561,12 +1605,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E20" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
+    <row r="20" spans="1:18" ht="24.95" customHeight="1" thickBot="1">
+      <c r="E20" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
@@ -1574,35 +1618,35 @@
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
     </row>
-    <row r="21" spans="1:14" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="50" t="s">
+    <row r="21" spans="1:18" ht="24.6" customHeight="1">
+      <c r="A21" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="52"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="25"/>
-      <c r="I21" s="50" t="s">
+      <c r="I21" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="52"/>
-    </row>
-    <row r="22" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="58"/>
+    </row>
+    <row r="22" spans="1:18" ht="26.1" customHeight="1">
       <c r="A22" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
+      <c r="C22" s="60"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="25"/>
       <c r="I22" s="23" t="s">
         <v>36</v>
@@ -1618,95 +1662,95 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="14.45" customHeight="1">
       <c r="A23" s="7">
         <v>0</v>
       </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="59"/>
-      <c r="E23" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="E23" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="25"/>
       <c r="I23" s="27" t="s">
         <v>35</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K23" s="28"/>
       <c r="L23" s="28" t="s">
         <v>38</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="14.45" customHeight="1">
       <c r="A24" s="7">
         <v>1</v>
       </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="59"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="25"/>
       <c r="I24" s="27" t="s">
         <v>35</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K24" s="28"/>
       <c r="L24" s="28" t="s">
         <v>38</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="7">
         <v>2</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="59"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="25"/>
       <c r="I25" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="9" t="s">
-        <v>76</v>
+      <c r="J25" s="41" t="s">
+        <v>73</v>
       </c>
       <c r="K25" s="28"/>
       <c r="L25" s="28" t="s">
         <v>38</v>
       </c>
       <c r="M25" s="43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="7">
         <v>3</v>
       </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="59"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
       <c r="H26" s="25"/>
       <c r="I26" s="27" t="s">
         <v>35</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="K26" s="28"/>
       <c r="L26" s="28" t="s">
@@ -1714,21 +1758,21 @@
       </c>
       <c r="M26" s="29"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18">
       <c r="A27" s="7">
         <v>4</v>
       </c>
-      <c r="B27" s="58"/>
-      <c r="C27" s="59"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
       <c r="H27" s="25"/>
       <c r="I27" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="41" t="s">
-        <v>62</v>
+      <c r="J27" s="28" t="s">
+        <v>68</v>
       </c>
       <c r="K27" s="28"/>
       <c r="L27" s="28" t="s">
@@ -1736,81 +1780,76 @@
       </c>
       <c r="M27" s="29"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18">
       <c r="A28" s="7">
         <v>5</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="59"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
       <c r="H28" s="25"/>
       <c r="I28" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="J28" s="41"/>
       <c r="K28" s="28"/>
       <c r="L28" s="28" t="s">
         <v>38</v>
       </c>
       <c r="M28" s="29"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18">
       <c r="A29" s="7">
         <v>6</v>
       </c>
-      <c r="B29" s="58"/>
-      <c r="C29" s="59"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
       <c r="H29" s="25"/>
       <c r="I29" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="28" t="s">
-        <v>64</v>
-      </c>
       <c r="K29" s="28"/>
       <c r="L29" s="28" t="s">
         <v>38</v>
       </c>
       <c r="M29" s="29"/>
     </row>
-    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" ht="15.75" thickBot="1">
       <c r="A30" s="7">
         <v>7</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="59"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
       <c r="H30" s="25"/>
       <c r="I30" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="31"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="31"/>
       <c r="L30" s="31" t="s">
         <v>38</v>
       </c>
       <c r="M30" s="32"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18">
       <c r="A31" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
+      <c r="C31" s="51"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
@@ -1818,17 +1857,17 @@
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
     </row>
-    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:18" ht="15.75" thickBot="1">
       <c r="A32" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
+      <c r="C32" s="53"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
@@ -1838,6 +1877,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="E20:G22"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
@@ -1854,14 +1901,6 @@
     <mergeCell ref="E23:G25"/>
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="I21:M21"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="E20:G22"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1871,23 +1910,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="38.54296875" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1">
       <c r="B2" s="36" t="s">
         <v>41</v>
       </c>
@@ -1898,21 +1937,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7">
       <c r="B3" s="44" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="39"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7">
       <c r="B4" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
     </row>
-    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" ht="15.75" thickBot="1">
       <c r="B5" s="35" t="s">
         <v>45</v>
       </c>
@@ -1920,8 +1959,8 @@
       <c r="D5" s="14"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" ht="15.75" thickBot="1"/>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1">
       <c r="B7" s="36" t="s">
         <v>42</v>
       </c>
@@ -1932,14 +1971,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7">
       <c r="B8" s="34">
         <v>1</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7">
       <c r="B9" s="42">
         <f>B8+1</f>
         <v>2</v>
@@ -1947,7 +1986,7 @@
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7">
       <c r="B10" s="42">
         <f t="shared" ref="B10:B18" si="0">B9+1</f>
         <v>3</v>
@@ -1955,7 +1994,7 @@
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7">
       <c r="B11" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1963,7 +2002,7 @@
       <c r="C11" s="39"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7">
       <c r="B12" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1971,7 +2010,7 @@
       <c r="C12" s="39"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7">
       <c r="B13" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1979,7 +2018,7 @@
       <c r="C13" s="39"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7">
       <c r="B14" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1987,7 +2026,7 @@
       <c r="C14" s="39"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7">
       <c r="B15" s="34">
         <f>B14+1</f>
         <v>8</v>
@@ -1995,7 +2034,7 @@
       <c r="C15" s="39"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7">
       <c r="B16" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2003,7 +2042,7 @@
       <c r="C16" s="39"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4">
       <c r="B17" s="42">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2011,7 +2050,7 @@
       <c r="C17" s="39"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1">
       <c r="B18" s="35">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2026,21 +2065,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2051,7 +2090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2062,7 +2101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2073,7 +2112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2084,13 +2123,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="45" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="45"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -2098,7 +2137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -2106,7 +2145,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -2114,7 +2153,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>53</v>
       </c>

</xml_diff>